<commit_message>
Update complete template excel for SELLING and PRODUCTION export flow
</commit_message>
<xml_diff>
--- a/public/export-templates/template_xuat_ban.xlsx
+++ b/public/export-templates/template_xuat_ban.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8337E4-535A-4CC9-A7C1-D163AA72A67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF6F4B-1732-49DA-9ACF-512ABF8DA45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
   </bookViews>
   <sheets>
     <sheet name="Template xuất bán" sheetId="2" r:id="rId1"/>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Hệ Thống Quản Lý Kho Vải </t>
-  </si>
   <si>
     <t>Loại xuất</t>
   </si>
@@ -71,9 +68,6 @@
     <t>PHIẾU XUẤT KHO - XUẤT BÁN</t>
   </si>
   <si>
-    <t>Số lượng</t>
-  </si>
-  <si>
     <t>Số thứ tự</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>SĐT người nhận</t>
+  </si>
+  <si>
+    <t>Hệ Thống Quản Lý Kho Vải FWMS</t>
+  </si>
+  <si>
+    <t>Số lượng cần xuất</t>
   </si>
 </sst>
 </file>
@@ -257,14 +257,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -274,25 +271,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,6 +328,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB4D399-E8CC-8E0F-C8A9-48DADB9D0881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="219075"/>
+          <a:ext cx="1222375" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -646,1234 +696,1248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6856CC1-CBFE-4ECB-B377-3A86D1DC5596}">
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="18.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="str">
-        <f>IF(B12&lt;&gt;"", COUNTA($B$12:B12), "")</f>
-        <v/>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="str">
-        <f>IF(B13&lt;&gt;"", COUNTA($B$12:B13), "")</f>
+      <c r="A13" s="10" t="str">
+        <f>IF(B13&lt;&gt;"", COUNTA($B$13:B13), "")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="str">
-        <f>IF(B14&lt;&gt;"", COUNTA($B$12:B14), "")</f>
+      <c r="A14" s="10" t="str">
+        <f>IF(B14&lt;&gt;"", COUNTA($B$13:B14), "")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="str">
-        <f>IF(B15&lt;&gt;"", COUNTA($B$12:B15), "")</f>
+      <c r="A15" s="10" t="str">
+        <f>IF(B15&lt;&gt;"", COUNTA($B$13:B15), "")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="str">
-        <f>IF(B16&lt;&gt;"", COUNTA($B$12:B16), "")</f>
+      <c r="A16" s="10" t="str">
+        <f>IF(B16&lt;&gt;"", COUNTA($B$13:B16), "")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="str">
-        <f>IF(B17&lt;&gt;"", COUNTA($B$12:B17), "")</f>
+      <c r="A17" s="10" t="str">
+        <f>IF(B17&lt;&gt;"", COUNTA($B$13:B17), "")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="str">
-        <f>IF(B18&lt;&gt;"", COUNTA($B$12:B18), "")</f>
+      <c r="A18" s="10" t="str">
+        <f>IF(B18&lt;&gt;"", COUNTA($B$13:B18), "")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="str">
-        <f>IF(B19&lt;&gt;"", COUNTA($B$12:B19), "")</f>
+      <c r="A19" s="10" t="str">
+        <f>IF(B19&lt;&gt;"", COUNTA($B$13:B19), "")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="str">
-        <f>IF(B20&lt;&gt;"", COUNTA($B$12:B20), "")</f>
+      <c r="A20" s="10" t="str">
+        <f>IF(B20&lt;&gt;"", COUNTA($B$13:B20), "")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="str">
-        <f>IF(B21&lt;&gt;"", COUNTA($B$12:B21), "")</f>
+      <c r="A21" s="10" t="str">
+        <f>IF(B21&lt;&gt;"", COUNTA($B$13:B21), "")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="str">
-        <f>IF(B22&lt;&gt;"", COUNTA($B$12:B22), "")</f>
+      <c r="A22" s="10" t="str">
+        <f>IF(B22&lt;&gt;"", COUNTA($B$13:B22), "")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="str">
-        <f>IF(B23&lt;&gt;"", COUNTA($B$12:B23), "")</f>
+      <c r="A23" s="10" t="str">
+        <f>IF(B23&lt;&gt;"", COUNTA($B$13:B23), "")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="str">
-        <f>IF(B24&lt;&gt;"", COUNTA($B$12:B24), "")</f>
+      <c r="A24" s="10" t="str">
+        <f>IF(B24&lt;&gt;"", COUNTA($B$13:B24), "")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="str">
-        <f>IF(B25&lt;&gt;"", COUNTA($B$12:B25), "")</f>
+      <c r="A25" s="10" t="str">
+        <f>IF(B25&lt;&gt;"", COUNTA($B$13:B25), "")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="str">
-        <f>IF(B26&lt;&gt;"", COUNTA($B$12:B26), "")</f>
+      <c r="A26" s="10" t="str">
+        <f>IF(B26&lt;&gt;"", COUNTA($B$13:B26), "")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="str">
-        <f>IF(B27&lt;&gt;"", COUNTA($B$12:B27), "")</f>
+      <c r="A27" s="10" t="str">
+        <f>IF(B27&lt;&gt;"", COUNTA($B$13:B27), "")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="str">
-        <f>IF(B28&lt;&gt;"", COUNTA($B$12:B28), "")</f>
+      <c r="A28" s="10" t="str">
+        <f>IF(B28&lt;&gt;"", COUNTA($B$13:B28), "")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="str">
-        <f>IF(B29&lt;&gt;"", COUNTA($B$12:B29), "")</f>
+      <c r="A29" s="10" t="str">
+        <f>IF(B29&lt;&gt;"", COUNTA($B$13:B29), "")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="str">
-        <f>IF(B30&lt;&gt;"", COUNTA($B$12:B30), "")</f>
+      <c r="A30" s="10" t="str">
+        <f>IF(B30&lt;&gt;"", COUNTA($B$13:B30), "")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="str">
-        <f>IF(B31&lt;&gt;"", COUNTA($B$12:B31), "")</f>
+      <c r="A31" s="10" t="str">
+        <f>IF(B31&lt;&gt;"", COUNTA($B$13:B31), "")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="str">
-        <f>IF(B32&lt;&gt;"", COUNTA($B$12:B32), "")</f>
+      <c r="A32" s="10" t="str">
+        <f>IF(B32&lt;&gt;"", COUNTA($B$13:B32), "")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="str">
-        <f>IF(B33&lt;&gt;"", COUNTA($B$12:B33), "")</f>
+      <c r="A33" s="10" t="str">
+        <f>IF(B33&lt;&gt;"", COUNTA($B$13:B33), "")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="str">
-        <f>IF(B34&lt;&gt;"", COUNTA($B$12:B34), "")</f>
+      <c r="A34" s="10" t="str">
+        <f>IF(B34&lt;&gt;"", COUNTA($B$13:B34), "")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="str">
-        <f>IF(B35&lt;&gt;"", COUNTA($B$12:B35), "")</f>
+      <c r="A35" s="10" t="str">
+        <f>IF(B35&lt;&gt;"", COUNTA($B$13:B35), "")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="str">
-        <f>IF(B36&lt;&gt;"", COUNTA($B$12:B36), "")</f>
+      <c r="A36" s="10" t="str">
+        <f>IF(B36&lt;&gt;"", COUNTA($B$13:B36), "")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="str">
-        <f>IF(B37&lt;&gt;"", COUNTA($B$12:B37), "")</f>
+      <c r="A37" s="10" t="str">
+        <f>IF(B37&lt;&gt;"", COUNTA($B$13:B37), "")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="str">
-        <f>IF(B38&lt;&gt;"", COUNTA($B$12:B38), "")</f>
+      <c r="A38" s="10" t="str">
+        <f>IF(B38&lt;&gt;"", COUNTA($B$13:B38), "")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="str">
-        <f>IF(B39&lt;&gt;"", COUNTA($B$12:B39), "")</f>
+      <c r="A39" s="10" t="str">
+        <f>IF(B39&lt;&gt;"", COUNTA($B$13:B39), "")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="str">
-        <f>IF(B40&lt;&gt;"", COUNTA($B$12:B40), "")</f>
+      <c r="A40" s="10" t="str">
+        <f>IF(B40&lt;&gt;"", COUNTA($B$13:B40), "")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="str">
-        <f>IF(B41&lt;&gt;"", COUNTA($B$12:B41), "")</f>
+      <c r="A41" s="10" t="str">
+        <f>IF(B41&lt;&gt;"", COUNTA($B$13:B41), "")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="str">
-        <f>IF(B42&lt;&gt;"", COUNTA($B$12:B42), "")</f>
+      <c r="A42" s="10" t="str">
+        <f>IF(B42&lt;&gt;"", COUNTA($B$13:B42), "")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="str">
-        <f>IF(B43&lt;&gt;"", COUNTA($B$12:B43), "")</f>
+      <c r="A43" s="10" t="str">
+        <f>IF(B43&lt;&gt;"", COUNTA($B$13:B43), "")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="str">
-        <f>IF(B44&lt;&gt;"", COUNTA($B$12:B44), "")</f>
+      <c r="A44" s="10" t="str">
+        <f>IF(B44&lt;&gt;"", COUNTA($B$13:B44), "")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="str">
-        <f>IF(B45&lt;&gt;"", COUNTA($B$12:B45), "")</f>
+      <c r="A45" s="10" t="str">
+        <f>IF(B45&lt;&gt;"", COUNTA($B$13:B45), "")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="str">
-        <f>IF(B46&lt;&gt;"", COUNTA($B$12:B46), "")</f>
+      <c r="A46" s="10" t="str">
+        <f>IF(B46&lt;&gt;"", COUNTA($B$13:B46), "")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="str">
-        <f>IF(B47&lt;&gt;"", COUNTA($B$12:B47), "")</f>
+      <c r="A47" s="10" t="str">
+        <f>IF(B47&lt;&gt;"", COUNTA($B$13:B47), "")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="str">
-        <f>IF(B48&lt;&gt;"", COUNTA($B$12:B48), "")</f>
+      <c r="A48" s="10" t="str">
+        <f>IF(B48&lt;&gt;"", COUNTA($B$13:B48), "")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="str">
-        <f>IF(B49&lt;&gt;"", COUNTA($B$12:B49), "")</f>
+      <c r="A49" s="10" t="str">
+        <f>IF(B49&lt;&gt;"", COUNTA($B$13:B49), "")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="str">
-        <f>IF(B50&lt;&gt;"", COUNTA($B$12:B50), "")</f>
+      <c r="A50" s="10" t="str">
+        <f>IF(B50&lt;&gt;"", COUNTA($B$13:B50), "")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="str">
-        <f>IF(B51&lt;&gt;"", COUNTA($B$12:B51), "")</f>
+      <c r="A51" s="10" t="str">
+        <f>IF(B51&lt;&gt;"", COUNTA($B$13:B51), "")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="str">
-        <f>IF(B52&lt;&gt;"", COUNTA($B$12:B52), "")</f>
+      <c r="A52" s="10" t="str">
+        <f>IF(B52&lt;&gt;"", COUNTA($B$13:B52), "")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="str">
-        <f>IF(B53&lt;&gt;"", COUNTA($B$12:B53), "")</f>
+      <c r="A53" s="10" t="str">
+        <f>IF(B53&lt;&gt;"", COUNTA($B$13:B53), "")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="str">
-        <f>IF(B54&lt;&gt;"", COUNTA($B$12:B54), "")</f>
+      <c r="A54" s="10" t="str">
+        <f>IF(B54&lt;&gt;"", COUNTA($B$13:B54), "")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="str">
-        <f>IF(B55&lt;&gt;"", COUNTA($B$12:B55), "")</f>
+      <c r="A55" s="10" t="str">
+        <f>IF(B55&lt;&gt;"", COUNTA($B$13:B55), "")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="str">
-        <f>IF(B56&lt;&gt;"", COUNTA($B$12:B56), "")</f>
+      <c r="A56" s="10" t="str">
+        <f>IF(B56&lt;&gt;"", COUNTA($B$13:B56), "")</f>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="str">
-        <f>IF(B57&lt;&gt;"", COUNTA($B$12:B57), "")</f>
+      <c r="A57" s="10" t="str">
+        <f>IF(B57&lt;&gt;"", COUNTA($B$13:B57), "")</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="str">
-        <f>IF(B58&lt;&gt;"", COUNTA($B$12:B58), "")</f>
+      <c r="A58" s="10" t="str">
+        <f>IF(B58&lt;&gt;"", COUNTA($B$13:B58), "")</f>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="str">
-        <f>IF(B59&lt;&gt;"", COUNTA($B$12:B59), "")</f>
+      <c r="A59" s="10" t="str">
+        <f>IF(B59&lt;&gt;"", COUNTA($B$13:B59), "")</f>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="str">
-        <f>IF(B60&lt;&gt;"", COUNTA($B$12:B60), "")</f>
+      <c r="A60" s="10" t="str">
+        <f>IF(B60&lt;&gt;"", COUNTA($B$13:B60), "")</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="str">
-        <f>IF(B61&lt;&gt;"", COUNTA($B$12:B61), "")</f>
+      <c r="A61" s="10" t="str">
+        <f>IF(B61&lt;&gt;"", COUNTA($B$13:B61), "")</f>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="str">
-        <f>IF(B62&lt;&gt;"", COUNTA($B$12:B62), "")</f>
+      <c r="A62" s="10" t="str">
+        <f>IF(B62&lt;&gt;"", COUNTA($B$13:B62), "")</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="str">
-        <f>IF(B63&lt;&gt;"", COUNTA($B$12:B63), "")</f>
+      <c r="A63" s="10" t="str">
+        <f>IF(B63&lt;&gt;"", COUNTA($B$13:B63), "")</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="str">
-        <f>IF(B64&lt;&gt;"", COUNTA($B$12:B64), "")</f>
+      <c r="A64" s="10" t="str">
+        <f>IF(B64&lt;&gt;"", COUNTA($B$13:B64), "")</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="str">
-        <f>IF(B65&lt;&gt;"", COUNTA($B$12:B65), "")</f>
+      <c r="A65" s="10" t="str">
+        <f>IF(B65&lt;&gt;"", COUNTA($B$13:B65), "")</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="str">
-        <f>IF(B66&lt;&gt;"", COUNTA($B$12:B66), "")</f>
+      <c r="A66" s="10" t="str">
+        <f>IF(B66&lt;&gt;"", COUNTA($B$13:B66), "")</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="str">
-        <f>IF(B67&lt;&gt;"", COUNTA($B$12:B67), "")</f>
+      <c r="A67" s="10" t="str">
+        <f>IF(B67&lt;&gt;"", COUNTA($B$13:B67), "")</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="str">
-        <f>IF(B68&lt;&gt;"", COUNTA($B$12:B68), "")</f>
+      <c r="A68" s="10" t="str">
+        <f>IF(B68&lt;&gt;"", COUNTA($B$13:B68), "")</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="str">
-        <f>IF(B69&lt;&gt;"", COUNTA($B$12:B69), "")</f>
+      <c r="A69" s="10" t="str">
+        <f>IF(B69&lt;&gt;"", COUNTA($B$13:B69), "")</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="str">
-        <f>IF(B70&lt;&gt;"", COUNTA($B$12:B70), "")</f>
+      <c r="A70" s="10" t="str">
+        <f>IF(B70&lt;&gt;"", COUNTA($B$13:B70), "")</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="str">
-        <f>IF(B71&lt;&gt;"", COUNTA($B$12:B71), "")</f>
+      <c r="A71" s="10" t="str">
+        <f>IF(B71&lt;&gt;"", COUNTA($B$13:B71), "")</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="str">
-        <f>IF(B72&lt;&gt;"", COUNTA($B$12:B72), "")</f>
+      <c r="A72" s="10" t="str">
+        <f>IF(B72&lt;&gt;"", COUNTA($B$13:B72), "")</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="str">
-        <f>IF(B73&lt;&gt;"", COUNTA($B$12:B73), "")</f>
+      <c r="A73" s="10" t="str">
+        <f>IF(B73&lt;&gt;"", COUNTA($B$13:B73), "")</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="str">
-        <f>IF(B74&lt;&gt;"", COUNTA($B$12:B74), "")</f>
+      <c r="A74" s="10" t="str">
+        <f>IF(B74&lt;&gt;"", COUNTA($B$13:B74), "")</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="str">
-        <f>IF(B75&lt;&gt;"", COUNTA($B$12:B75), "")</f>
+      <c r="A75" s="10" t="str">
+        <f>IF(B75&lt;&gt;"", COUNTA($B$13:B75), "")</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14" t="str">
-        <f>IF(B76&lt;&gt;"", COUNTA($B$12:B76), "")</f>
+      <c r="A76" s="10" t="str">
+        <f>IF(B76&lt;&gt;"", COUNTA($B$13:B76), "")</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="str">
-        <f>IF(B77&lt;&gt;"", COUNTA($B$12:B77), "")</f>
+      <c r="A77" s="10" t="str">
+        <f>IF(B77&lt;&gt;"", COUNTA($B$13:B77), "")</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="str">
-        <f>IF(B78&lt;&gt;"", COUNTA($B$12:B78), "")</f>
+      <c r="A78" s="10" t="str">
+        <f>IF(B78&lt;&gt;"", COUNTA($B$13:B78), "")</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="str">
-        <f>IF(B79&lt;&gt;"", COUNTA($B$12:B79), "")</f>
+      <c r="A79" s="10" t="str">
+        <f>IF(B79&lt;&gt;"", COUNTA($B$13:B79), "")</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="str">
-        <f>IF(B80&lt;&gt;"", COUNTA($B$12:B80), "")</f>
+      <c r="A80" s="10" t="str">
+        <f>IF(B80&lt;&gt;"", COUNTA($B$13:B80), "")</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="str">
-        <f>IF(B81&lt;&gt;"", COUNTA($B$12:B81), "")</f>
+      <c r="A81" s="10" t="str">
+        <f>IF(B81&lt;&gt;"", COUNTA($B$13:B81), "")</f>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="str">
-        <f>IF(B82&lt;&gt;"", COUNTA($B$12:B82), "")</f>
+      <c r="A82" s="10" t="str">
+        <f>IF(B82&lt;&gt;"", COUNTA($B$13:B82), "")</f>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="str">
-        <f>IF(B83&lt;&gt;"", COUNTA($B$12:B83), "")</f>
+      <c r="A83" s="10" t="str">
+        <f>IF(B83&lt;&gt;"", COUNTA($B$13:B83), "")</f>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="str">
-        <f>IF(B84&lt;&gt;"", COUNTA($B$12:B84), "")</f>
+      <c r="A84" s="10" t="str">
+        <f>IF(B84&lt;&gt;"", COUNTA($B$13:B84), "")</f>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="str">
-        <f>IF(B85&lt;&gt;"", COUNTA($B$12:B85), "")</f>
+      <c r="A85" s="10" t="str">
+        <f>IF(B85&lt;&gt;"", COUNTA($B$13:B85), "")</f>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14" t="str">
-        <f>IF(B86&lt;&gt;"", COUNTA($B$12:B86), "")</f>
+      <c r="A86" s="10" t="str">
+        <f>IF(B86&lt;&gt;"", COUNTA($B$13:B86), "")</f>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="str">
-        <f>IF(B87&lt;&gt;"", COUNTA($B$12:B87), "")</f>
+      <c r="A87" s="10" t="str">
+        <f>IF(B87&lt;&gt;"", COUNTA($B$13:B87), "")</f>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="str">
-        <f>IF(B88&lt;&gt;"", COUNTA($B$12:B88), "")</f>
+      <c r="A88" s="10" t="str">
+        <f>IF(B88&lt;&gt;"", COUNTA($B$13:B88), "")</f>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="str">
-        <f>IF(B89&lt;&gt;"", COUNTA($B$12:B89), "")</f>
+      <c r="A89" s="10" t="str">
+        <f>IF(B89&lt;&gt;"", COUNTA($B$13:B89), "")</f>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="str">
-        <f>IF(B90&lt;&gt;"", COUNTA($B$12:B90), "")</f>
+      <c r="A90" s="10" t="str">
+        <f>IF(B90&lt;&gt;"", COUNTA($B$13:B90), "")</f>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="str">
-        <f>IF(B91&lt;&gt;"", COUNTA($B$12:B91), "")</f>
+      <c r="A91" s="10" t="str">
+        <f>IF(B91&lt;&gt;"", COUNTA($B$13:B91), "")</f>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="str">
-        <f>IF(B92&lt;&gt;"", COUNTA($B$12:B92), "")</f>
+      <c r="A92" s="10" t="str">
+        <f>IF(B92&lt;&gt;"", COUNTA($B$13:B92), "")</f>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="str">
-        <f>IF(B93&lt;&gt;"", COUNTA($B$12:B93), "")</f>
+      <c r="A93" s="10" t="str">
+        <f>IF(B93&lt;&gt;"", COUNTA($B$13:B93), "")</f>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="str">
-        <f>IF(B94&lt;&gt;"", COUNTA($B$12:B94), "")</f>
+      <c r="A94" s="10" t="str">
+        <f>IF(B94&lt;&gt;"", COUNTA($B$13:B94), "")</f>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="str">
-        <f>IF(B95&lt;&gt;"", COUNTA($B$12:B95), "")</f>
+      <c r="A95" s="10" t="str">
+        <f>IF(B95&lt;&gt;"", COUNTA($B$13:B95), "")</f>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14" t="str">
-        <f>IF(B96&lt;&gt;"", COUNTA($B$12:B96), "")</f>
+      <c r="A96" s="10" t="str">
+        <f>IF(B96&lt;&gt;"", COUNTA($B$13:B96), "")</f>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="str">
-        <f>IF(B97&lt;&gt;"", COUNTA($B$12:B97), "")</f>
+      <c r="A97" s="10" t="str">
+        <f>IF(B97&lt;&gt;"", COUNTA($B$13:B97), "")</f>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="str">
-        <f>IF(B98&lt;&gt;"", COUNTA($B$12:B98), "")</f>
+      <c r="A98" s="10" t="str">
+        <f>IF(B98&lt;&gt;"", COUNTA($B$13:B98), "")</f>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14" t="str">
-        <f>IF(B99&lt;&gt;"", COUNTA($B$12:B99), "")</f>
+      <c r="A99" s="10" t="str">
+        <f>IF(B99&lt;&gt;"", COUNTA($B$13:B99), "")</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14" t="str">
-        <f>IF(B100&lt;&gt;"", COUNTA($B$12:B100), "")</f>
+      <c r="A100" s="10" t="str">
+        <f>IF(B100&lt;&gt;"", COUNTA($B$13:B100), "")</f>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="14" t="str">
-        <f>IF(B101&lt;&gt;"", COUNTA($B$12:B101), "")</f>
+      <c r="A101" s="10" t="str">
+        <f>IF(B101&lt;&gt;"", COUNTA($B$13:B101), "")</f>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="str">
-        <f>IF(B102&lt;&gt;"", COUNTA($B$12:B102), "")</f>
+      <c r="A102" s="10" t="str">
+        <f>IF(B102&lt;&gt;"", COUNTA($B$13:B102), "")</f>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14" t="str">
-        <f>IF(B103&lt;&gt;"", COUNTA($B$12:B103), "")</f>
+      <c r="A103" s="10" t="str">
+        <f>IF(B103&lt;&gt;"", COUNTA($B$13:B103), "")</f>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="str">
-        <f>IF(B104&lt;&gt;"", COUNTA($B$12:B104), "")</f>
+      <c r="A104" s="10" t="str">
+        <f>IF(B104&lt;&gt;"", COUNTA($B$13:B104), "")</f>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="str">
-        <f>IF(B105&lt;&gt;"", COUNTA($B$12:B105), "")</f>
+      <c r="A105" s="10" t="str">
+        <f>IF(B105&lt;&gt;"", COUNTA($B$13:B105), "")</f>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14" t="str">
-        <f>IF(B106&lt;&gt;"", COUNTA($B$12:B106), "")</f>
+      <c r="A106" s="10" t="str">
+        <f>IF(B106&lt;&gt;"", COUNTA($B$13:B106), "")</f>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="14" t="str">
-        <f>IF(B107&lt;&gt;"", COUNTA($B$12:B107), "")</f>
+      <c r="A107" s="10" t="str">
+        <f>IF(B107&lt;&gt;"", COUNTA($B$13:B107), "")</f>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="14" t="str">
-        <f>IF(B108&lt;&gt;"", COUNTA($B$12:B108), "")</f>
+      <c r="A108" s="10" t="str">
+        <f>IF(B108&lt;&gt;"", COUNTA($B$13:B108), "")</f>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="14" t="str">
-        <f>IF(B109&lt;&gt;"", COUNTA($B$12:B109), "")</f>
+      <c r="A109" s="10" t="str">
+        <f>IF(B109&lt;&gt;"", COUNTA($B$13:B109), "")</f>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="str">
-        <f>IF(B110&lt;&gt;"", COUNTA($B$12:B110), "")</f>
+      <c r="A110" s="10" t="str">
+        <f>IF(B110&lt;&gt;"", COUNTA($B$13:B110), "")</f>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="str">
-        <f>IF(B111&lt;&gt;"", COUNTA($B$12:B111), "")</f>
+      <c r="A111" s="10" t="str">
+        <f>IF(B111&lt;&gt;"", COUNTA($B$13:B111), "")</f>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="str">
-        <f>IF(B112&lt;&gt;"", COUNTA($B$12:B112), "")</f>
+      <c r="A112" s="10" t="str">
+        <f>IF(B112&lt;&gt;"", COUNTA($B$13:B112), "")</f>
         <v/>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="str">
-        <f>IF(B113&lt;&gt;"", COUNTA($B$12:B113), "")</f>
+      <c r="A113" s="10" t="str">
+        <f>IF(B113&lt;&gt;"", COUNTA($B$13:B113), "")</f>
         <v/>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="14" t="str">
-        <f>IF(B114&lt;&gt;"", COUNTA($B$12:B114), "")</f>
+      <c r="A114" s="10" t="str">
+        <f>IF(B114&lt;&gt;"", COUNTA($B$13:B114), "")</f>
         <v/>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14" t="str">
-        <f>IF(B115&lt;&gt;"", COUNTA($B$12:B115), "")</f>
+      <c r="A115" s="10" t="str">
+        <f>IF(B115&lt;&gt;"", COUNTA($B$13:B115), "")</f>
         <v/>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="str">
-        <f>IF(B116&lt;&gt;"", COUNTA($B$12:B116), "")</f>
+      <c r="A116" s="10" t="str">
+        <f>IF(B116&lt;&gt;"", COUNTA($B$13:B116), "")</f>
         <v/>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="str">
-        <f>IF(B117&lt;&gt;"", COUNTA($B$12:B117), "")</f>
+      <c r="A117" s="10" t="str">
+        <f>IF(B117&lt;&gt;"", COUNTA($B$13:B117), "")</f>
         <v/>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="str">
-        <f>IF(B118&lt;&gt;"", COUNTA($B$12:B118), "")</f>
+      <c r="A118" s="10" t="str">
+        <f>IF(B118&lt;&gt;"", COUNTA($B$13:B118), "")</f>
         <v/>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="str">
-        <f>IF(B119&lt;&gt;"", COUNTA($B$12:B119), "")</f>
+      <c r="A119" s="10" t="str">
+        <f>IF(B119&lt;&gt;"", COUNTA($B$13:B119), "")</f>
         <v/>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14" t="str">
-        <f>IF(B120&lt;&gt;"", COUNTA($B$12:B120), "")</f>
+      <c r="A120" s="10" t="str">
+        <f>IF(B120&lt;&gt;"", COUNTA($B$13:B120), "")</f>
         <v/>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14" t="str">
-        <f>IF(B121&lt;&gt;"", COUNTA($B$12:B121), "")</f>
+      <c r="A121" s="10" t="str">
+        <f>IF(B121&lt;&gt;"", COUNTA($B$13:B121), "")</f>
         <v/>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14" t="str">
-        <f>IF(B122&lt;&gt;"", COUNTA($B$12:B122), "")</f>
+      <c r="A122" s="10" t="str">
+        <f>IF(B122&lt;&gt;"", COUNTA($B$13:B122), "")</f>
         <v/>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="14" t="str">
-        <f>IF(B123&lt;&gt;"", COUNTA($B$12:B123), "")</f>
+      <c r="A123" s="10" t="str">
+        <f>IF(B123&lt;&gt;"", COUNTA($B$13:B123), "")</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14" t="str">
-        <f>IF(B124&lt;&gt;"", COUNTA($B$12:B124), "")</f>
+      <c r="A124" s="10" t="str">
+        <f>IF(B124&lt;&gt;"", COUNTA($B$13:B124), "")</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14" t="str">
-        <f>IF(B125&lt;&gt;"", COUNTA($B$12:B125), "")</f>
+      <c r="A125" s="10" t="str">
+        <f>IF(B125&lt;&gt;"", COUNTA($B$13:B125), "")</f>
         <v/>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="14" t="str">
-        <f>IF(B126&lt;&gt;"", COUNTA($B$12:B126), "")</f>
+      <c r="A126" s="10" t="str">
+        <f>IF(B126&lt;&gt;"", COUNTA($B$13:B126), "")</f>
         <v/>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="str">
-        <f>IF(B127&lt;&gt;"", COUNTA($B$12:B127), "")</f>
+      <c r="A127" s="10" t="str">
+        <f>IF(B127&lt;&gt;"", COUNTA($B$13:B127), "")</f>
         <v/>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="14" t="str">
-        <f>IF(B128&lt;&gt;"", COUNTA($B$12:B128), "")</f>
+      <c r="A128" s="10" t="str">
+        <f>IF(B128&lt;&gt;"", COUNTA($B$13:B128), "")</f>
         <v/>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14" t="str">
-        <f>IF(B129&lt;&gt;"", COUNTA($B$12:B129), "")</f>
+      <c r="A129" s="10" t="str">
+        <f>IF(B129&lt;&gt;"", COUNTA($B$13:B129), "")</f>
         <v/>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14" t="str">
-        <f>IF(B130&lt;&gt;"", COUNTA($B$12:B130), "")</f>
+      <c r="A130" s="10" t="str">
+        <f>IF(B130&lt;&gt;"", COUNTA($B$13:B130), "")</f>
         <v/>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14" t="str">
-        <f>IF(B131&lt;&gt;"", COUNTA($B$12:B131), "")</f>
+      <c r="A131" s="10" t="str">
+        <f>IF(B131&lt;&gt;"", COUNTA($B$13:B131), "")</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14" t="str">
-        <f>IF(B132&lt;&gt;"", COUNTA($B$12:B132), "")</f>
+      <c r="A132" s="10" t="str">
+        <f>IF(B132&lt;&gt;"", COUNTA($B$13:B132), "")</f>
         <v/>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14" t="str">
-        <f>IF(B133&lt;&gt;"", COUNTA($B$12:B133), "")</f>
+      <c r="A133" s="10" t="str">
+        <f>IF(B133&lt;&gt;"", COUNTA($B$13:B133), "")</f>
         <v/>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="14" t="str">
-        <f>IF(B134&lt;&gt;"", COUNTA($B$12:B134), "")</f>
+      <c r="A134" s="10" t="str">
+        <f>IF(B134&lt;&gt;"", COUNTA($B$13:B134), "")</f>
         <v/>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14" t="str">
-        <f>IF(B135&lt;&gt;"", COUNTA($B$12:B135), "")</f>
+      <c r="A135" s="10" t="str">
+        <f>IF(B135&lt;&gt;"", COUNTA($B$13:B135), "")</f>
         <v/>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14" t="str">
-        <f>IF(B136&lt;&gt;"", COUNTA($B$12:B136), "")</f>
+      <c r="A136" s="10" t="str">
+        <f>IF(B136&lt;&gt;"", COUNTA($B$13:B136), "")</f>
         <v/>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14" t="str">
-        <f>IF(B137&lt;&gt;"", COUNTA($B$12:B137), "")</f>
+      <c r="A137" s="10" t="str">
+        <f>IF(B137&lt;&gt;"", COUNTA($B$13:B137), "")</f>
         <v/>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14" t="str">
-        <f>IF(B138&lt;&gt;"", COUNTA($B$12:B138), "")</f>
+      <c r="A138" s="10" t="str">
+        <f>IF(B138&lt;&gt;"", COUNTA($B$13:B138), "")</f>
         <v/>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14" t="str">
-        <f>IF(B139&lt;&gt;"", COUNTA($B$12:B139), "")</f>
+      <c r="A139" s="10" t="str">
+        <f>IF(B139&lt;&gt;"", COUNTA($B$13:B139), "")</f>
         <v/>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14" t="str">
-        <f>IF(B140&lt;&gt;"", COUNTA($B$12:B140), "")</f>
+      <c r="A140" s="10" t="str">
+        <f>IF(B140&lt;&gt;"", COUNTA($B$13:B140), "")</f>
         <v/>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14" t="str">
-        <f>IF(B141&lt;&gt;"", COUNTA($B$12:B141), "")</f>
+      <c r="A141" s="10" t="str">
+        <f>IF(B141&lt;&gt;"", COUNTA($B$13:B141), "")</f>
         <v/>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14" t="str">
-        <f>IF(B142&lt;&gt;"", COUNTA($B$12:B142), "")</f>
+      <c r="A142" s="10" t="str">
+        <f>IF(B142&lt;&gt;"", COUNTA($B$13:B142), "")</f>
         <v/>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14" t="str">
-        <f>IF(B143&lt;&gt;"", COUNTA($B$12:B143), "")</f>
+      <c r="A143" s="10" t="str">
+        <f>IF(B143&lt;&gt;"", COUNTA($B$13:B143), "")</f>
         <v/>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="14" t="str">
-        <f>IF(B144&lt;&gt;"", COUNTA($B$12:B144), "")</f>
+      <c r="A144" s="10" t="str">
+        <f>IF(B144&lt;&gt;"", COUNTA($B$13:B144), "")</f>
         <v/>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14" t="str">
-        <f>IF(B145&lt;&gt;"", COUNTA($B$12:B145), "")</f>
+      <c r="A145" s="10" t="str">
+        <f>IF(B145&lt;&gt;"", COUNTA($B$13:B145), "")</f>
         <v/>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14" t="str">
-        <f>IF(B146&lt;&gt;"", COUNTA($B$12:B146), "")</f>
+      <c r="A146" s="10" t="str">
+        <f>IF(B146&lt;&gt;"", COUNTA($B$13:B146), "")</f>
         <v/>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14" t="str">
-        <f>IF(B147&lt;&gt;"", COUNTA($B$12:B147), "")</f>
+      <c r="A147" s="10" t="str">
+        <f>IF(B147&lt;&gt;"", COUNTA($B$13:B147), "")</f>
         <v/>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14" t="str">
-        <f>IF(B148&lt;&gt;"", COUNTA($B$12:B148), "")</f>
+      <c r="A148" s="10" t="str">
+        <f>IF(B148&lt;&gt;"", COUNTA($B$13:B148), "")</f>
         <v/>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="14" t="str">
-        <f>IF(B149&lt;&gt;"", COUNTA($B$12:B149), "")</f>
+      <c r="A149" s="10" t="str">
+        <f>IF(B149&lt;&gt;"", COUNTA($B$13:B149), "")</f>
         <v/>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14" t="str">
-        <f>IF(B150&lt;&gt;"", COUNTA($B$12:B150), "")</f>
+      <c r="A150" s="10" t="str">
+        <f>IF(B150&lt;&gt;"", COUNTA($B$13:B150), "")</f>
         <v/>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14" t="str">
-        <f>IF(B151&lt;&gt;"", COUNTA($B$12:B151), "")</f>
+      <c r="A151" s="10" t="str">
+        <f>IF(B151&lt;&gt;"", COUNTA($B$13:B151), "")</f>
         <v/>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14" t="str">
-        <f>IF(B152&lt;&gt;"", COUNTA($B$12:B152), "")</f>
+      <c r="A152" s="10" t="str">
+        <f>IF(B152&lt;&gt;"", COUNTA($B$13:B152), "")</f>
         <v/>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14" t="str">
-        <f>IF(B153&lt;&gt;"", COUNTA($B$12:B153), "")</f>
+      <c r="A153" s="10" t="str">
+        <f>IF(B153&lt;&gt;"", COUNTA($B$13:B153), "")</f>
         <v/>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14" t="str">
-        <f>IF(B154&lt;&gt;"", COUNTA($B$12:B154), "")</f>
+      <c r="A154" s="10" t="str">
+        <f>IF(B154&lt;&gt;"", COUNTA($B$13:B154), "")</f>
         <v/>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14" t="str">
-        <f>IF(B155&lt;&gt;"", COUNTA($B$12:B155), "")</f>
+      <c r="A155" s="10" t="str">
+        <f>IF(B155&lt;&gt;"", COUNTA($B$13:B155), "")</f>
         <v/>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14" t="str">
-        <f>IF(B156&lt;&gt;"", COUNTA($B$12:B156), "")</f>
+      <c r="A156" s="10" t="str">
+        <f>IF(B156&lt;&gt;"", COUNTA($B$13:B156), "")</f>
         <v/>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="14" t="str">
-        <f>IF(B157&lt;&gt;"", COUNTA($B$12:B157), "")</f>
+      <c r="A157" s="10" t="str">
+        <f>IF(B157&lt;&gt;"", COUNTA($B$13:B157), "")</f>
         <v/>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14" t="str">
-        <f>IF(B158&lt;&gt;"", COUNTA($B$12:B158), "")</f>
+      <c r="A158" s="10" t="str">
+        <f>IF(B158&lt;&gt;"", COUNTA($B$13:B158), "")</f>
         <v/>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14" t="str">
-        <f>IF(B159&lt;&gt;"", COUNTA($B$12:B159), "")</f>
+      <c r="A159" s="10" t="str">
+        <f>IF(B159&lt;&gt;"", COUNTA($B$13:B159), "")</f>
         <v/>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14" t="str">
-        <f>IF(B160&lt;&gt;"", COUNTA($B$12:B160), "")</f>
+      <c r="A160" s="10" t="str">
+        <f>IF(B160&lt;&gt;"", COUNTA($B$13:B160), "")</f>
         <v/>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14" t="str">
-        <f>IF(B161&lt;&gt;"", COUNTA($B$12:B161), "")</f>
+      <c r="A161" s="10" t="str">
+        <f>IF(B161&lt;&gt;"", COUNTA($B$13:B161), "")</f>
         <v/>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14" t="str">
-        <f>IF(B162&lt;&gt;"", COUNTA($B$12:B162), "")</f>
+      <c r="A162" s="10" t="str">
+        <f>IF(B162&lt;&gt;"", COUNTA($B$13:B162), "")</f>
         <v/>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="14" t="str">
-        <f>IF(B163&lt;&gt;"", COUNTA($B$12:B163), "")</f>
+      <c r="A163" s="10" t="str">
+        <f>IF(B163&lt;&gt;"", COUNTA($B$13:B163), "")</f>
         <v/>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="14" t="str">
-        <f>IF(B164&lt;&gt;"", COUNTA($B$12:B164), "")</f>
+      <c r="A164" s="10" t="str">
+        <f>IF(B164&lt;&gt;"", COUNTA($B$13:B164), "")</f>
         <v/>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="14" t="str">
-        <f>IF(B165&lt;&gt;"", COUNTA($B$12:B165), "")</f>
+      <c r="A165" s="10" t="str">
+        <f>IF(B165&lt;&gt;"", COUNTA($B$13:B165), "")</f>
         <v/>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="14" t="str">
-        <f>IF(B166&lt;&gt;"", COUNTA($B$12:B166), "")</f>
+      <c r="A166" s="10" t="str">
+        <f>IF(B166&lt;&gt;"", COUNTA($B$13:B166), "")</f>
         <v/>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="14" t="str">
-        <f>IF(B167&lt;&gt;"", COUNTA($B$12:B167), "")</f>
+      <c r="A167" s="10" t="str">
+        <f>IF(B167&lt;&gt;"", COUNTA($B$13:B167), "")</f>
         <v/>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="14" t="str">
-        <f>IF(B168&lt;&gt;"", COUNTA($B$12:B168), "")</f>
+      <c r="A168" s="10" t="str">
+        <f>IF(B168&lt;&gt;"", COUNTA($B$13:B168), "")</f>
         <v/>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14" t="str">
-        <f>IF(B169&lt;&gt;"", COUNTA($B$12:B169), "")</f>
+      <c r="A169" s="10" t="str">
+        <f>IF(B169&lt;&gt;"", COUNTA($B$13:B169), "")</f>
         <v/>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="14" t="str">
-        <f>IF(B170&lt;&gt;"", COUNTA($B$12:B170), "")</f>
+      <c r="A170" s="10" t="str">
+        <f>IF(B170&lt;&gt;"", COUNTA($B$13:B170), "")</f>
         <v/>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14" t="str">
-        <f>IF(B171&lt;&gt;"", COUNTA($B$12:B171), "")</f>
+      <c r="A171" s="10" t="str">
+        <f>IF(B171&lt;&gt;"", COUNTA($B$13:B171), "")</f>
         <v/>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14" t="str">
-        <f>IF(B172&lt;&gt;"", COUNTA($B$12:B172), "")</f>
+      <c r="A172" s="10" t="str">
+        <f>IF(B172&lt;&gt;"", COUNTA($B$13:B172), "")</f>
         <v/>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="14" t="str">
-        <f>IF(B173&lt;&gt;"", COUNTA($B$12:B173), "")</f>
+      <c r="A173" s="10" t="str">
+        <f>IF(B173&lt;&gt;"", COUNTA($B$13:B173), "")</f>
         <v/>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14" t="str">
-        <f>IF(B174&lt;&gt;"", COUNTA($B$12:B174), "")</f>
+      <c r="A174" s="10" t="str">
+        <f>IF(B174&lt;&gt;"", COUNTA($B$13:B174), "")</f>
         <v/>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14" t="str">
-        <f>IF(B175&lt;&gt;"", COUNTA($B$12:B175), "")</f>
+      <c r="A175" s="10" t="str">
+        <f>IF(B175&lt;&gt;"", COUNTA($B$13:B175), "")</f>
         <v/>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14" t="str">
-        <f>IF(B176&lt;&gt;"", COUNTA($B$12:B176), "")</f>
+      <c r="A176" s="10" t="str">
+        <f>IF(B176&lt;&gt;"", COUNTA($B$13:B176), "")</f>
         <v/>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14" t="str">
-        <f>IF(B177&lt;&gt;"", COUNTA($B$12:B177), "")</f>
+      <c r="A177" s="10" t="str">
+        <f>IF(B177&lt;&gt;"", COUNTA($B$13:B177), "")</f>
         <v/>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14" t="str">
-        <f>IF(B178&lt;&gt;"", COUNTA($B$12:B178), "")</f>
+      <c r="A178" s="10" t="str">
+        <f>IF(B178&lt;&gt;"", COUNTA($B$13:B178), "")</f>
         <v/>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="14" t="str">
-        <f>IF(B179&lt;&gt;"", COUNTA($B$12:B179), "")</f>
+      <c r="A179" s="10" t="str">
+        <f>IF(B179&lt;&gt;"", COUNTA($B$13:B179), "")</f>
         <v/>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14" t="str">
-        <f>IF(B180&lt;&gt;"", COUNTA($B$12:B180), "")</f>
+      <c r="A180" s="10" t="str">
+        <f>IF(B180&lt;&gt;"", COUNTA($B$13:B180), "")</f>
         <v/>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14" t="str">
-        <f>IF(B181&lt;&gt;"", COUNTA($B$12:B181), "")</f>
+      <c r="A181" s="10" t="str">
+        <f>IF(B181&lt;&gt;"", COUNTA($B$13:B181), "")</f>
         <v/>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="14" t="str">
-        <f>IF(B182&lt;&gt;"", COUNTA($B$12:B182), "")</f>
+      <c r="A182" s="10" t="str">
+        <f>IF(B182&lt;&gt;"", COUNTA($B$13:B182), "")</f>
         <v/>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14" t="str">
-        <f>IF(B183&lt;&gt;"", COUNTA($B$12:B183), "")</f>
+      <c r="A183" s="10" t="str">
+        <f>IF(B183&lt;&gt;"", COUNTA($B$13:B183), "")</f>
         <v/>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="14" t="str">
-        <f>IF(B184&lt;&gt;"", COUNTA($B$12:B184), "")</f>
+      <c r="A184" s="10" t="str">
+        <f>IF(B184&lt;&gt;"", COUNTA($B$13:B184), "")</f>
         <v/>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14" t="str">
-        <f>IF(B185&lt;&gt;"", COUNTA($B$12:B185), "")</f>
+      <c r="A185" s="10" t="str">
+        <f>IF(B185&lt;&gt;"", COUNTA($B$13:B185), "")</f>
         <v/>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14" t="str">
-        <f>IF(B186&lt;&gt;"", COUNTA($B$12:B186), "")</f>
+      <c r="A186" s="10" t="str">
+        <f>IF(B186&lt;&gt;"", COUNTA($B$13:B186), "")</f>
         <v/>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14" t="str">
-        <f>IF(B187&lt;&gt;"", COUNTA($B$12:B187), "")</f>
+      <c r="A187" s="10" t="str">
+        <f>IF(B187&lt;&gt;"", COUNTA($B$13:B187), "")</f>
         <v/>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14" t="str">
-        <f>IF(B188&lt;&gt;"", COUNTA($B$12:B188), "")</f>
+      <c r="A188" s="10" t="str">
+        <f>IF(B188&lt;&gt;"", COUNTA($B$13:B188), "")</f>
         <v/>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14" t="str">
-        <f>IF(B189&lt;&gt;"", COUNTA($B$12:B189), "")</f>
+      <c r="A189" s="10" t="str">
+        <f>IF(B189&lt;&gt;"", COUNTA($B$13:B189), "")</f>
         <v/>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14" t="str">
-        <f>IF(B190&lt;&gt;"", COUNTA($B$12:B190), "")</f>
+      <c r="A190" s="10" t="str">
+        <f>IF(B190&lt;&gt;"", COUNTA($B$13:B190), "")</f>
         <v/>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="14" t="str">
-        <f>IF(B191&lt;&gt;"", COUNTA($B$12:B191), "")</f>
+      <c r="A191" s="10" t="str">
+        <f>IF(B191&lt;&gt;"", COUNTA($B$13:B191), "")</f>
         <v/>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14" t="str">
-        <f>IF(B192&lt;&gt;"", COUNTA($B$12:B192), "")</f>
+      <c r="A192" s="10" t="str">
+        <f>IF(B192&lt;&gt;"", COUNTA($B$13:B192), "")</f>
         <v/>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14" t="str">
-        <f>IF(B193&lt;&gt;"", COUNTA($B$12:B193), "")</f>
+      <c r="A193" s="10" t="str">
+        <f>IF(B193&lt;&gt;"", COUNTA($B$13:B193), "")</f>
         <v/>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14" t="str">
-        <f>IF(B194&lt;&gt;"", COUNTA($B$12:B194), "")</f>
+      <c r="A194" s="10" t="str">
+        <f>IF(B194&lt;&gt;"", COUNTA($B$13:B194), "")</f>
         <v/>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14" t="str">
-        <f>IF(B195&lt;&gt;"", COUNTA($B$12:B195), "")</f>
+      <c r="A195" s="10" t="str">
+        <f>IF(B195&lt;&gt;"", COUNTA($B$13:B195), "")</f>
         <v/>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14" t="str">
-        <f>IF(B196&lt;&gt;"", COUNTA($B$12:B196), "")</f>
+      <c r="A196" s="10" t="str">
+        <f>IF(B196&lt;&gt;"", COUNTA($B$13:B196), "")</f>
         <v/>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14" t="str">
-        <f>IF(B197&lt;&gt;"", COUNTA($B$12:B197), "")</f>
+      <c r="A197" s="10" t="str">
+        <f>IF(B197&lt;&gt;"", COUNTA($B$13:B197), "")</f>
         <v/>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14" t="str">
-        <f>IF(B198&lt;&gt;"", COUNTA($B$12:B198), "")</f>
+      <c r="A198" s="10" t="str">
+        <f>IF(B198&lt;&gt;"", COUNTA($B$13:B198), "")</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14" t="str">
-        <f>IF(B199&lt;&gt;"", COUNTA($B$12:B199), "")</f>
+      <c r="A199" s="10" t="str">
+        <f>IF(B199&lt;&gt;"", COUNTA($B$13:B199), "")</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14" t="str">
-        <f>IF(B200&lt;&gt;"", COUNTA($B$12:B200), "")</f>
+      <c r="A200" s="10" t="str">
+        <f>IF(B200&lt;&gt;"", COUNTA($B$13:B200), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="10" t="str">
+        <f>IF(B201&lt;&gt;"", COUNTA($B$13:B201), "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="U0jpct7o/ftzmrKAtMXtsXCvWD0JCFD4xjfruym/OMLdFP6ckIOBq1B54IcqKzgg7xK6ZdPaZ59AGsVGl5B69g==" saltValue="uyW0pWOuKxqGPgw/L4/RuQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="A11:C200">
+  <sheetProtection algorithmName="SHA-512" hashValue="VbCws/R5WJrN9ubLkR8vOkDZ3xnl/zRoLwmjFR6a76b2PWkQ+biWbc8BhMmk7MlsKjudBupvxkdz4TNcEBxPkA==" saltValue="4QRp4WYmHviAwG8j1Jbo1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <conditionalFormatting sqref="A12:C201">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>A11&lt;&gt;""</formula>
+      <formula>A12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C200" xr:uid="{DADA5064-923E-4BF9-B12C-20271FEF6702}">
-      <formula1>OR(B12="", AND(ISNUMBER(C12), C12&gt;0, B12&lt;&gt;""))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C201" xr:uid="{DADA5064-923E-4BF9-B12C-20271FEF6702}">
+      <formula1>OR(B13="", AND(ISNUMBER(C13), C13&gt;0, B13&lt;&gt;""))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change label of export type from PRODUCTION to INTERNAL
</commit_message>
<xml_diff>
--- a/public/export-templates/template_xuat_ban.xlsx
+++ b/public/export-templates/template_xuat_ban.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisd\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF6F4B-1732-49DA-9ACF-512ABF8DA45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A56F72E-0224-49A9-9D67-FF54C36B1003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
   </bookViews>
   <sheets>
     <sheet name="Template xuất bán" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Loại xuất</t>
   </si>
@@ -47,22 +47,10 @@
     <t>Lí do xuất</t>
   </si>
   <si>
-    <t>Xuất bán cho các bên khác</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tên người nhận </t>
   </si>
   <si>
-    <t>Hiếu Trần</t>
-  </si>
-  <si>
     <t>Địa chỉ người nhận</t>
-  </si>
-  <si>
-    <t>đường 123, quận ABC</t>
-  </si>
-  <si>
-    <t>0786110802</t>
   </si>
   <si>
     <t>PHIẾU XUẤT KHO - XUẤT BÁN</t>
@@ -275,25 +263,25 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,15 +323,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>539115</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -366,8 +354,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="219075"/>
-          <a:ext cx="1222375" cy="733425"/>
+          <a:off x="200026" y="47626"/>
+          <a:ext cx="819149" cy="491489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,25 +687,27 @@
   <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="10" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>13</v>
+    <row r="1" spans="1:3" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="C1" s="14"/>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -727,7 +717,7 @@
     <row r="4" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="14"/>
     </row>
@@ -748,33 +738,25 @@
       <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -782,13 +764,13 @@
     </row>
     <row r="12" spans="1:3" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,7 +1908,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VbCws/R5WJrN9ubLkR8vOkDZ3xnl/zRoLwmjFR6a76b2PWkQ+biWbc8BhMmk7MlsKjudBupvxkdz4TNcEBxPkA==" saltValue="4QRp4WYmHviAwG8j1Jbo1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="y8Ncih9DW9Kgzraf7Rlczm0caWg0igRdOzOBqAdh8X5AnNJ5ryLGXS0k0SlhKeTKbFEcy+cn91TdJDD47Vd3ZQ==" saltValue="xfE7xm80n96qqFK4F+PkcQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A12:C201">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>A12&lt;&gt;""</formula>

</xml_diff>